<commit_message>
Add comments to code; Update main to organize packages onto trucks;
</commit_message>
<xml_diff>
--- a/WGUPS Package File.xlsx
+++ b/WGUPS Package File.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miguel.dehoyos\Downloads\C950\New Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\CVRPTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7D6FC3F-E74F-4587-BEDF-A00C8FAE7100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D78036-9F84-4799-9AB6-CEC142831C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -326,7 +326,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>929640</xdr:colOff>
+      <xdr:colOff>882015</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>115169</xdr:rowOff>
     </xdr:to>
@@ -635,21 +635,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="3.77734375" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" customWidth="1"/>
-    <col min="6" max="6" width="7" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" customWidth="1"/>
-    <col min="8" max="8" width="39.77734375" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
@@ -661,7 +661,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
@@ -673,7 +673,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -685,7 +685,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
@@ -698,7 +698,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -709,7 +709,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>48</v>
       </c>
@@ -721,7 +721,7 @@
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="3" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>45</v>
       </c>
@@ -747,7 +747,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>1</v>
       </c>
@@ -771,7 +771,7 @@
       </c>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>2</v>
       </c>
@@ -795,7 +795,7 @@
       </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>3</v>
       </c>
@@ -821,7 +821,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>4</v>
       </c>
@@ -845,7 +845,7 @@
       </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>5</v>
       </c>
@@ -869,7 +869,7 @@
       </c>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>6</v>
       </c>
@@ -895,7 +895,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>7</v>
       </c>
@@ -919,7 +919,7 @@
       </c>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>8</v>
       </c>
@@ -943,7 +943,7 @@
       </c>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>9</v>
       </c>
@@ -969,7 +969,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>10</v>
       </c>
@@ -993,7 +993,7 @@
       </c>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>11</v>
       </c>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>12</v>
       </c>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>13</v>
       </c>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>14</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>15</v>
       </c>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>16</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>17</v>
       </c>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>18</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>19</v>
       </c>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>20</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>21</v>
       </c>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>22</v>
       </c>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>23</v>
       </c>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>24</v>
       </c>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>25</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>26</v>
       </c>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>27</v>
       </c>
@@ -1411,7 +1411,7 @@
       </c>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>28</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>29</v>
       </c>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>30</v>
       </c>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>31</v>
       </c>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>32</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>33</v>
       </c>
@@ -1559,7 +1559,7 @@
       </c>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>34</v>
       </c>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>35</v>
       </c>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>36</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>37</v>
       </c>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>38</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>39</v>
       </c>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="H47" s="4"/>
     </row>
-    <row r="48" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>40</v>
       </c>
@@ -1744,15 +1744,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Course_x0020_title xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
@@ -1799,6 +1790,15 @@
     <_x0033_rdPartyCertVendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2312,14 +2312,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E77ABB-EDCD-4FE8-A23F-B30F5B1F6DEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ACC0CE6-074E-44A2-B54E-38496285A228}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2333,10 +2325,35 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="1f707338-ea0f-4fe5-baee-59b996692b22"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E77ABB-EDCD-4FE8-A23F-B30F5B1F6DEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5214019-7508-47A8-9FC8-EDBE31C095C4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5214019-7508-47A8-9FC8-EDBE31C095C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
+    <ds:schemaRef ds:uri="1f707338-ea0f-4fe5-baee-59b996692b22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>